<commit_message>
Schema changed. Implemented existing form of agreements and pay contract. Updated file DBSettings.xlsx, ReportTemplates.xlsx
</commit_message>
<xml_diff>
--- a/DatabaseUpdate/ExcelFiles/DBSettings.xlsx
+++ b/DatabaseUpdate/ExcelFiles/DBSettings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -55,16 +55,16 @@
     <x:t>2</x:t>
   </x:si>
   <x:si>
-    <x:t>CurrentLpuName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Больница №1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Название текущего ЛПУ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3</x:t>
+    <x:t>OrgName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Государственное бюджетное образовательное учреждение высшего профессионального образования «Российский национальный исследовательский медицинский университет имени Н.И.Пирогова» Министерства здравоохранения Российской Федерации</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Полное название ЛПУ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
   </x:si>
   <x:si>
     <x:t>NotificationServiceAddress</x:t>
@@ -74,6 +74,129 @@
   </x:si>
   <x:si>
     <x:t>Адрес сервиса оповещений</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OrgOKPO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11223444</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ОКПО ЛПУ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OrgShortName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ГБОУ ВПО РНИМУ им. Н.И. Пирогова МЗ РФ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Сокращенное название ЛПУ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NIKIName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Научно-исследовательский клинический институт педиатрии им. академика Ю.Е. Вельтищева ГБОУ ВПО РНИМУ им. Н.И. Пирогова МЗ РФ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Научно-исследовательском клиническом институте педиатрии им. академика Ю.Е. Вельтищева ГБОУ ВПО РНИМУ им. Н.И. Пирогова МЗ РФ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Название обособленного структурного подразделения НИКИ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DirectorFullName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Школьникова Мария Александровна</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Школьниковой Марии Александровны</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Директор НИКИ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PayContractLicense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17 марта 2014 года № 52</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Доверенность на оказание платных услуг</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NIKIAddress</x:t>
+  </x:si>
+  <x:si>
+    <x:t>125412, г. Москва, ул. Талдомская, д. 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Адрес НИКИ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OrgAddress</x:t>
+  </x:si>
+  <x:si>
+    <x:t>117997, г. Москва, ул. Островитянова, д. 1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Юридический адрес</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DirectorShortName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Школьникова М.А.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NIKIShortName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Научно-исследовательский клинический институт педиатрии</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Научно-исследовательском клиническом институте педиатрии</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Сокращенное название обособленного структурного подразделения НИКИ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ChildAge</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Возраст, старше которого человек считается взрослым</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -431,7 +554,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:H4"/>
+  <x:dimension ref="A1:H14"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -482,7 +605,7 @@
         <x:v>36526</x:v>
       </x:c>
       <x:c r="H2" s="1">
-        <x:v>72686</x:v>
+        <x:v>2958100</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:8">
@@ -504,7 +627,7 @@
         <x:v>36526</x:v>
       </x:c>
       <x:c r="H3" s="1">
-        <x:v>72686</x:v>
+        <x:v>2958100</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:8">
@@ -526,7 +649,235 @@
         <x:v>36526</x:v>
       </x:c>
       <x:c r="H4" s="1">
-        <x:v>72686</x:v>
+        <x:v>2958100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:8">
+      <x:c r="A5" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s"/>
+      <x:c r="E5" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s"/>
+      <x:c r="G5" s="1">
+        <x:v>36526</x:v>
+      </x:c>
+      <x:c r="H5" s="1">
+        <x:v>2958100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:8">
+      <x:c r="A6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s"/>
+      <x:c r="E6" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s"/>
+      <x:c r="G6" s="1">
+        <x:v>36526</x:v>
+      </x:c>
+      <x:c r="H6" s="1">
+        <x:v>2958100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:8">
+      <x:c r="A7" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s"/>
+      <x:c r="G7" s="1">
+        <x:v>36526</x:v>
+      </x:c>
+      <x:c r="H7" s="1">
+        <x:v>2958100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:8">
+      <x:c r="A8" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s"/>
+      <x:c r="G8" s="1">
+        <x:v>36526</x:v>
+      </x:c>
+      <x:c r="H8" s="1">
+        <x:v>2958100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:8">
+      <x:c r="A9" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s"/>
+      <x:c r="E9" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s"/>
+      <x:c r="G9" s="1">
+        <x:v>36526</x:v>
+      </x:c>
+      <x:c r="H9" s="1">
+        <x:v>2958100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:8">
+      <x:c r="A10" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s"/>
+      <x:c r="E10" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s"/>
+      <x:c r="G10" s="1">
+        <x:v>36526</x:v>
+      </x:c>
+      <x:c r="H10" s="1">
+        <x:v>2958100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:8">
+      <x:c r="A11" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s"/>
+      <x:c r="E11" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s"/>
+      <x:c r="G11" s="1">
+        <x:v>36526</x:v>
+      </x:c>
+      <x:c r="H11" s="1">
+        <x:v>2958100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:8">
+      <x:c r="A12" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s"/>
+      <x:c r="G12" s="1">
+        <x:v>36526</x:v>
+      </x:c>
+      <x:c r="H12" s="1">
+        <x:v>2958100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:8">
+      <x:c r="A13" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s"/>
+      <x:c r="G13" s="1">
+        <x:v>36526</x:v>
+      </x:c>
+      <x:c r="H13" s="1">
+        <x:v>2958100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:8">
+      <x:c r="A14" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s"/>
+      <x:c r="E14" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s"/>
+      <x:c r="G14" s="1">
+        <x:v>36526</x:v>
+      </x:c>
+      <x:c r="H14" s="1">
+        <x:v>2958100</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Schema changed. Updated excel files.
Add statistics report for analyze schedule work
</commit_message>
<xml_diff>
--- a/DatabaseUpdate/ExcelFiles/DBSettings.xlsx
+++ b/DatabaseUpdate/ExcelFiles/DBSettings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -40,160 +40,100 @@
     <x:t>EndDateTime</x:t>
   </x:si>
   <x:si>
-    <x:t>1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DefaultRecordTypeTime</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8:00 - 12:00, 12:00 - 17:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Время, проставляемое в расписании по умолчанию для новых типов услуг</x:t>
-  </x:si>
-  <x:si>
     <x:t>2</x:t>
   </x:si>
   <x:si>
     <x:t>OrgName</x:t>
   </x:si>
   <x:si>
-    <x:t>Государственное бюджетное образовательное учреждение высшего профессионального образования «Российский национальный исследовательский медицинский университет имени Н.И.Пирогова» Министерства здравоохранения Российской Федерации</x:t>
+    <x:t>КЛИНИКА</x:t>
   </x:si>
   <x:si>
     <x:t>Полное название ЛПУ</x:t>
   </x:si>
   <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NotificationServiceAddress</x:t>
+  </x:si>
+  <x:si>
+    <x:t>net.tcp://localhost:8733/NotificationServiceEngine</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Адрес сервиса оповещений</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OrgOKPO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11223444</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ОКПО ЛПУ</x:t>
+  </x:si>
+  <x:si>
     <x:t>5</x:t>
   </x:si>
   <x:si>
-    <x:t>NotificationServiceAddress</x:t>
-  </x:si>
-  <x:si>
-    <x:t>net.tcp://localhost:8733/NotificationServiceEngine</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Адрес сервиса оповещений</x:t>
+    <x:t>OrgShortName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Сокращенное название ЛПУ</x:t>
   </x:si>
   <x:si>
     <x:t>7</x:t>
   </x:si>
   <x:si>
-    <x:t>OrgOKPO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11223444</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ОКПО ЛПУ</x:t>
+    <x:t>DirectorFullName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>РУКОВОДИТЕЛЬ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Руководитель</x:t>
   </x:si>
   <x:si>
     <x:t>8</x:t>
   </x:si>
   <x:si>
-    <x:t>OrgShortName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ГБОУ ВПО РНИМУ им. Н.И. Пирогова МЗ РФ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Сокращенное название ЛПУ</x:t>
+    <x:t>PayContractLicense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ДОВЕРЕННОСТЬ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Доверенность на оказание платных услуг</x:t>
   </x:si>
   <x:si>
     <x:t>10</x:t>
   </x:si>
   <x:si>
-    <x:t>NIKIName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Научно-исследовательский клинический институт педиатрии им. академика Ю.Е. Вельтищева ГБОУ ВПО РНИМУ им. Н.И. Пирогова МЗ РФ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Научно-исследовательском клиническом институте педиатрии им. академика Ю.Е. Вельтищева ГБОУ ВПО РНИМУ им. Н.И. Пирогова МЗ РФ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Название обособленного структурного подразделения НИКИ</x:t>
+    <x:t>OrgAddress</x:t>
+  </x:si>
+  <x:si>
+    <x:t>АДРЕС</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Юридический адрес</x:t>
   </x:si>
   <x:si>
     <x:t>11</x:t>
   </x:si>
   <x:si>
-    <x:t>DirectorFullName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Школьникова Мария Александровна</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Школьниковой Марии Александровны</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Директор НИКИ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PayContractLicense</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17 марта 2014 года № 52</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Доверенность на оказание платных услуг</x:t>
+    <x:t>DirectorShortName</x:t>
   </x:si>
   <x:si>
     <x:t>13</x:t>
   </x:si>
   <x:si>
-    <x:t>NIKIAddress</x:t>
-  </x:si>
-  <x:si>
-    <x:t>125412, г. Москва, ул. Талдомская, д. 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Адрес НИКИ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>14</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OrgAddress</x:t>
-  </x:si>
-  <x:si>
-    <x:t>117997, г. Москва, ул. Островитянова, д. 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Юридический адрес</x:t>
+    <x:t>ChildAge</x:t>
   </x:si>
   <x:si>
     <x:t>15</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DirectorShortName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Школьникова М.А.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NIKIShortName</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Научно-исследовательский клинический институт педиатрии</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Научно-исследовательском клиническом институте педиатрии</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Сокращенное название обособленного структурного подразделения НИКИ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ChildAge</x:t>
   </x:si>
   <x:si>
     <x:t>Возраст, старше которого человек считается взрослым</x:t>
@@ -554,7 +494,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:H14"/>
+  <x:dimension ref="A1:H10"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -596,11 +536,9 @@
       <x:c r="C2" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s"/>
       <x:c r="E2" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s"/>
       <x:c r="G2" s="1">
         <x:v>36526</x:v>
       </x:c>
@@ -618,11 +556,9 @@
       <x:c r="C3" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s"/>
       <x:c r="E3" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="F3" s="0" t="s"/>
       <x:c r="G3" s="1">
         <x:v>36526</x:v>
       </x:c>
@@ -640,11 +576,9 @@
       <x:c r="C4" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D4" s="0" t="s"/>
       <x:c r="E4" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="F4" s="0" t="s"/>
       <x:c r="G4" s="1">
         <x:v>36526</x:v>
       </x:c>
@@ -660,13 +594,11 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="D5" s="0" t="s"/>
-      <x:c r="E5" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s"/>
       <x:c r="G5" s="1">
         <x:v>36526</x:v>
       </x:c>
@@ -676,19 +608,20 @@
     </x:row>
     <x:row r="6" spans="1:8">
       <x:c r="A6" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B6" s="0" t="s">
+      <x:c r="C6" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="C6" s="0" t="s">
+      <x:c r="D6" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="D6" s="0" t="s"/>
-      <x:c r="E6" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="F6" s="0" t="s"/>
       <x:c r="G6" s="1">
         <x:v>36526</x:v>
       </x:c>
@@ -698,21 +631,17 @@
     </x:row>
     <x:row r="7" spans="1:8">
       <x:c r="A7" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="B7" s="0" t="s">
+      <x:c r="C7" s="0" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="C7" s="0" t="s">
+      <x:c r="E7" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="F7" s="0" t="s"/>
       <x:c r="G7" s="1">
         <x:v>36526</x:v>
       </x:c>
@@ -722,21 +651,17 @@
     </x:row>
     <x:row r="8" spans="1:8">
       <x:c r="A8" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="B8" s="0" t="s">
+      <x:c r="E8" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="E8" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="F8" s="0" t="s"/>
       <x:c r="G8" s="1">
         <x:v>36526</x:v>
       </x:c>
@@ -746,19 +671,20 @@
     </x:row>
     <x:row r="9" spans="1:8">
       <x:c r="A9" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s"/>
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="F9" s="0" t="s"/>
+        <x:v>26</x:v>
+      </x:c>
       <x:c r="G9" s="1">
         <x:v>36526</x:v>
       </x:c>
@@ -768,115 +694,21 @@
     </x:row>
     <x:row r="10" spans="1:8">
       <x:c r="A10" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s"/>
+        <x:v>39</x:v>
+      </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="F10" s="0" t="s"/>
+        <x:v>40</x:v>
+      </x:c>
       <x:c r="G10" s="1">
         <x:v>36526</x:v>
       </x:c>
       <x:c r="H10" s="1">
-        <x:v>2958100</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:8">
-      <x:c r="A11" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="C11" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="D11" s="0" t="s"/>
-      <x:c r="E11" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="F11" s="0" t="s"/>
-      <x:c r="G11" s="1">
-        <x:v>36526</x:v>
-      </x:c>
-      <x:c r="H11" s="1">
-        <x:v>2958100</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:8">
-      <x:c r="A12" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="C12" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="E12" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="F12" s="0" t="s"/>
-      <x:c r="G12" s="1">
-        <x:v>36526</x:v>
-      </x:c>
-      <x:c r="H12" s="1">
-        <x:v>2958100</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:8">
-      <x:c r="A13" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="B13" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="C13" s="0" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="D13" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="E13" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="F13" s="0" t="s"/>
-      <x:c r="G13" s="1">
-        <x:v>36526</x:v>
-      </x:c>
-      <x:c r="H13" s="1">
-        <x:v>2958100</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:8">
-      <x:c r="A14" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="B14" s="0" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="C14" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="D14" s="0" t="s"/>
-      <x:c r="E14" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="F14" s="0" t="s"/>
-      <x:c r="G14" s="1">
-        <x:v>36526</x:v>
-      </x:c>
-      <x:c r="H14" s="1">
         <x:v>2958100</x:v>
       </x:c>
     </x:row>

</xml_diff>